<commit_message>
added array pattern on every simulation
</commit_message>
<xml_diff>
--- a/written/presentation/excels/MontecarloPower.xlsx
+++ b/written/presentation/excels/MontecarloPower.xlsx
@@ -2020,11 +2020,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1567838768"/>
-        <c:axId val="-1567836048"/>
+        <c:axId val="111008592"/>
+        <c:axId val="111006960"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1567838768"/>
+        <c:axId val="111008592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="70"/>
@@ -2138,12 +2138,12 @@
             <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1567836048"/>
+        <c:crossAx val="111006960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1567836048"/>
+        <c:axId val="111006960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2256,7 +2256,7 @@
             <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1567838768"/>
+        <c:crossAx val="111008592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3220,7 +3220,7 @@
   <dimension ref="A1:E71"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T12" sqref="T12"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>